<commit_message>
Inactivité le week end Ajout d'un log recorder pour logguer l'historique en cas d'erreur
</commit_message>
<xml_diff>
--- a/src/main/resources/boursorama.xlsx
+++ b/src/main/resources/boursorama.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="5430"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="boursorama" sheetId="1" r:id="rId1"/>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +467,9 @@
     <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
+    <row r="6" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>